<commit_message>
New Changes with the old project
</commit_message>
<xml_diff>
--- a/src/Deployment/road_inspection_database.xlsx
+++ b/src/Deployment/road_inspection_database.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Road_Inspection_Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,23 +28,13 @@
     <font>
       <b val="1"/>
     </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="002c3e50"/>
-        <bgColor rgb="002c3e50"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -67,7 +57,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -435,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,22 +523,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DET_20250921_090951_1</t>
+          <t>DET_20250927_080330_1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-21 09:09:51</t>
+          <t>2025-09-27 08:03:30</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sit Tumakuru Main Road </t>
+          <t>Tumakuru</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">BH Road </t>
+          <t>Mg road</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -563,7 +553,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0.822</v>
+        <v>0.819</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -585,14 +575,10 @@
           <t>To Be Decided</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Please Fix it </t>
-        </is>
-      </c>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Municipal Administrator</t>
+          <t>Jnaneshwari P</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -608,22 +594,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DET_20250921_090951_4</t>
+          <t>DET_20250927_080330_2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-21 09:09:51</t>
+          <t>2025-09-27 08:03:30</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sit Tumakuru Main Road </t>
+          <t>Tumakuru</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">BH Road </t>
+          <t>Mg road</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -634,11 +620,11 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>alligator-crack</t>
+          <t>pothole</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0.333</v>
+        <v>0.287</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -652,7 +638,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Standard Repair Method</t>
+          <t>Hot Mix Asphalt Patching</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -660,14 +646,10 @@
           <t>To Be Decided</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Please Fix it </t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Municipal Administrator</t>
+          <t>Jnaneshwari P</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -676,159 +658,9 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Q3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>DET_20250921_090951_5</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-09-21 09:09:51</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Sit Tumakuru Main Road </t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BH Road </t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>12.9716</v>
-      </c>
-      <c r="F4" t="n">
-        <v>77.5946</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>alligator-crack</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>0.313</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Standard Repair Method</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>To Be Decided</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Please Fix it </t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Municipal Administrator</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>In Progress</t>
-        </is>
-      </c>
-      <c r="P4" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>DET_20250921_090951_6</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2025-09-21 09:09:51</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Sit Tumakuru Main Road </t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BH Road </t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>12.9716</v>
-      </c>
-      <c r="F5" t="n">
-        <v>77.5946</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>alligator-crack</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>0.285</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Standard Repair Method</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>To Be Decided</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Please Fix it </t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Municipal Administrator</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Reported</t>
-        </is>
-      </c>
-      <c r="P5" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>